<commit_message>
Working, added horizontal scrollbars
</commit_message>
<xml_diff>
--- a/Test Data/To Map.xlsx
+++ b/Test Data/To Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whittlj2.WHS\github\Mapping_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whittlj2.WHS\github\Mapping_Tool\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35232CDB-E585-401E-BE27-6068D22462C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BE1C85-A5F9-427E-A0AC-634253FB814A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6225" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4050" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4050" uniqueCount="1313">
   <si>
     <t>PBS_CODE</t>
   </si>
@@ -3970,6 +3970,9 @@
   </si>
   <si>
     <t>DuoResp Spiromax</t>
+  </si>
+  <si>
+    <t>budesonide + formoterol budesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterolbudesonide + formoterol</t>
   </si>
 </sst>
 </file>
@@ -4305,14 +4308,14 @@
   <dimension ref="A1:F1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -4346,7 +4349,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>1312</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -24560,8 +24563,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>